<commit_message>
Created gopro rename program
Signed-off-by: Albert <wensinlor@gmail.com>
</commit_message>
<xml_diff>
--- a/Meeting_Materials/Jayden_Yap_Jia_Yu_Application_to_Employ_Research_Assistants_Form.xlsx
+++ b/Meeting_Materials/Jayden_Yap_Jia_Yu_Application_to_Employ_Research_Assistants_Form.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albertlor\Academic\URECA\Meeting_Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B17B42-DACD-41D0-AB89-70B5C8735AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E98F61-C1B4-42FB-915C-46240D97AD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Job Title:</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Data Collection in Construction Site</t>
-  </si>
-  <si>
-    <t>30/6/2023</t>
   </si>
   <si>
     <t>MAE</t>
@@ -929,7 +926,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1097,7 +1094,7 @@
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="57">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="E9" s="58"/>
       <c r="F9" s="58"/>
@@ -1107,8 +1104,8 @@
       <c r="J9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="59" t="s">
-        <v>29</v>
+      <c r="K9" s="59">
+        <v>45138</v>
       </c>
       <c r="L9" s="56"/>
       <c r="M9" s="4"/>
@@ -1138,7 +1135,7 @@
       </c>
       <c r="C11" s="14"/>
       <c r="G11" s="41">
-        <v>36.75</v>
+        <v>20.25</v>
       </c>
       <c r="H11" s="41"/>
       <c r="I11" s="41"/>
@@ -1222,7 +1219,7 @@
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="60">
-        <v>147</v>
+        <v>81</v>
       </c>
       <c r="I16" s="60"/>
       <c r="J16" s="9"/>
@@ -1286,7 +1283,7 @@
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" s="62"/>
       <c r="H20" s="62"/>
@@ -1322,7 +1319,7 @@
       <c r="D22" s="10"/>
       <c r="E22" s="9"/>
       <c r="F22" s="62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22" s="62"/>
       <c r="H22" s="62"/>
@@ -1331,7 +1328,7 @@
         <v>9</v>
       </c>
       <c r="K22" s="62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L22" s="62"/>
       <c r="M22" s="4"/>

</xml_diff>